<commit_message>
finished marking ground truth
</commit_message>
<xml_diff>
--- a/freqdistwordsLinkedin.xlsx
+++ b/freqdistwordsLinkedin.xlsx
@@ -8303,7 +8303,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -9613,7 +9613,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>32</v>
       </c>
@@ -11858,7 +11858,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>239</v>
       </c>
@@ -15171,7 +15171,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
         <v>418</v>
       </c>
@@ -20038,7 +20038,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="797" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="797" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A797" t="s">
         <v>637</v>
       </c>
@@ -29634,7 +29634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="1431" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1431" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1431" t="s">
         <v>1070</v>
       </c>
@@ -35242,7 +35242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1799" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1799" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1799" t="s">
         <v>1240</v>
       </c>
@@ -35259,7 +35259,7 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="1800" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1800" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1800" t="s">
         <v>1241</v>
       </c>
@@ -35276,7 +35276,7 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="1801" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1801" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1801" t="s">
         <v>1242</v>
       </c>
@@ -37367,7 +37367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1933" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1933" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1933" t="s">
         <v>1266</v>
       </c>
@@ -37927,7 +37927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1970" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1970" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1970" t="s">
         <v>1303</v>
       </c>
@@ -40200,7 +40200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2121" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2121" t="s">
         <v>1381</v>
       </c>
@@ -40532,7 +40532,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="2143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2143" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2143" t="s">
         <v>1402</v>
       </c>
@@ -42765,7 +42765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2292" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2292" t="s">
         <v>1495</v>
       </c>
@@ -44249,7 +44249,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2389" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2389" t="s">
         <v>1555</v>
       </c>
@@ -44266,7 +44266,7 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="2390" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2390" t="s">
         <v>1556</v>
       </c>
@@ -46972,7 +46972,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="2567" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2567" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2567" t="s">
         <v>1637</v>
       </c>
@@ -47121,7 +47121,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="2577" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2577" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2577" t="s">
         <v>1647</v>
       </c>
@@ -47442,7 +47442,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="2598" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2598" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2598" t="s">
         <v>1668</v>
       </c>
@@ -49720,7 +49720,7 @@
         <v>2477</v>
       </c>
     </row>
-    <row r="2750" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2750" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2750" t="s">
         <v>1734</v>
       </c>
@@ -49912,7 +49912,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2762" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2762" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2762" t="s">
         <v>1746</v>
       </c>
@@ -49960,7 +49960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2765" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2765" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2765" t="s">
         <v>1749</v>
       </c>
@@ -51141,7 +51141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2847" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2847" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2847" t="s">
         <v>1831</v>
       </c>
@@ -53642,7 +53642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3013" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3013" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3013" t="s">
         <v>1954</v>
       </c>
@@ -54066,11 +54066,9 @@
   </sheetData>
   <autoFilter ref="A1:F3041">
     <filterColumn colId="4">
-      <filters>
-        <filter val="l"/>
-        <filter val="t"/>
-        <filter val="x"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>